<commit_message>
started to add TNT - added svg export too
</commit_message>
<xml_diff>
--- a/results/tables/Error_types_table.xlsx
+++ b/results/tables/Error_types_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G160"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4799,7 +4799,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4818,19 +4818,19 @@
         </is>
       </c>
       <c r="E144">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F144">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G144">
-        <v>72.72727272727273</v>
+        <v>61.11111111111111</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4849,19 +4849,19 @@
         </is>
       </c>
       <c r="E145">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F145">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G145">
-        <v>18.18181818181818</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -4880,29 +4880,29 @@
         </is>
       </c>
       <c r="E146">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F146">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G146">
-        <v>9.090909090909092</v>
+        <v>5.555555555555555</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>100 Australian species</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4911,29 +4911,29 @@
         </is>
       </c>
       <c r="E147">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="F147">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G147">
-        <v>78.18181818181819</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>100 Australian species</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4942,55 +4942,55 @@
         </is>
       </c>
       <c r="E148">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F148">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G148">
-        <v>18.18181818181818</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>100 Australian species</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Genus and species wrong</t>
+          <t>Genus and species correct</t>
         </is>
       </c>
       <c r="E149">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="F149">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G149">
-        <v>3.636363636363636</v>
+        <v>85.41666666666666</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -5000,28 +5000,28 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Genus and species correct</t>
+          <t>Genus correct, species wrong</t>
         </is>
       </c>
       <c r="E150">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F150">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G150">
-        <v>66.66666666666666</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>VSEARCH</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Rottnest</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -5031,17 +5031,17 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Genus correct, species wrong</t>
+          <t>Genus and species wrong</t>
         </is>
       </c>
       <c r="E151">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F151">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G151">
-        <v>33.33333333333333</v>
+        <v>2.083333333333333</v>
       </c>
     </row>
     <row r="152">
@@ -5052,12 +5052,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -5066,13 +5066,13 @@
         </is>
       </c>
       <c r="E152">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="F152">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="G152">
-        <v>46.15384615384615</v>
+        <v>72.72727272727273</v>
       </c>
     </row>
     <row r="153">
@@ -5083,12 +5083,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -5097,13 +5097,13 @@
         </is>
       </c>
       <c r="E153">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F153">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="G153">
-        <v>46.15384615384615</v>
+        <v>18.18181818181818</v>
       </c>
     </row>
     <row r="154">
@@ -5114,12 +5114,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -5128,13 +5128,13 @@
         </is>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F154">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="G154">
-        <v>7.692307692307693</v>
+        <v>9.090909090909092</v>
       </c>
     </row>
     <row r="155">
@@ -5145,12 +5145,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -5159,13 +5159,13 @@
         </is>
       </c>
       <c r="E155">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F155">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G155">
-        <v>76.47058823529412</v>
+        <v>78.18181818181819</v>
       </c>
     </row>
     <row r="156">
@@ -5176,12 +5176,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -5190,13 +5190,13 @@
         </is>
       </c>
       <c r="E156">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F156">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G156">
-        <v>17.64705882352941</v>
+        <v>18.18181818181818</v>
       </c>
     </row>
     <row r="157">
@@ -5207,12 +5207,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -5221,13 +5221,13 @@
         </is>
       </c>
       <c r="E157">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F157">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G157">
-        <v>5.88235294117647</v>
+        <v>3.636363636363636</v>
       </c>
     </row>
     <row r="158">
@@ -5238,12 +5238,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -5252,13 +5252,13 @@
         </is>
       </c>
       <c r="E158">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="F158">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="G158">
-        <v>87.17948717948718</v>
+        <v>66.66666666666666</v>
       </c>
     </row>
     <row r="159">
@@ -5269,12 +5269,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -5283,13 +5283,13 @@
         </is>
       </c>
       <c r="E159">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F159">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="G159">
-        <v>8.974358974358974</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row r="160">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5310,16 +5310,264 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
+          <t>Genus and species correct</t>
+        </is>
+      </c>
+      <c r="E160">
+        <v>6</v>
+      </c>
+      <c r="F160">
+        <v>13</v>
+      </c>
+      <c r="G160">
+        <v>46.15384615384615</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Genus correct, species wrong</t>
+        </is>
+      </c>
+      <c r="E161">
+        <v>6</v>
+      </c>
+      <c r="F161">
+        <v>13</v>
+      </c>
+      <c r="G161">
+        <v>46.15384615384615</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
           <t>Genus and species wrong</t>
         </is>
       </c>
-      <c r="E160">
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>13</v>
+      </c>
+      <c r="G162">
+        <v>7.692307692307693</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Genus and species correct</t>
+        </is>
+      </c>
+      <c r="E163">
+        <v>52</v>
+      </c>
+      <c r="F163">
+        <v>68</v>
+      </c>
+      <c r="G163">
+        <v>76.47058823529412</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Genus correct, species wrong</t>
+        </is>
+      </c>
+      <c r="E164">
+        <v>12</v>
+      </c>
+      <c r="F164">
+        <v>68</v>
+      </c>
+      <c r="G164">
+        <v>17.64705882352941</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Genus and species wrong</t>
+        </is>
+      </c>
+      <c r="E165">
+        <v>4</v>
+      </c>
+      <c r="F165">
+        <v>68</v>
+      </c>
+      <c r="G165">
+        <v>5.88235294117647</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Genus and species correct</t>
+        </is>
+      </c>
+      <c r="E166">
+        <v>68</v>
+      </c>
+      <c r="F166">
+        <v>78</v>
+      </c>
+      <c r="G166">
+        <v>87.17948717948718</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Genus correct, species wrong</t>
+        </is>
+      </c>
+      <c r="E167">
+        <v>7</v>
+      </c>
+      <c r="F167">
+        <v>78</v>
+      </c>
+      <c r="G167">
+        <v>8.974358974358974</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Genus and species wrong</t>
+        </is>
+      </c>
+      <c r="E168">
         <v>3</v>
       </c>
-      <c r="F160">
+      <c r="F168">
         <v>78</v>
       </c>
-      <c r="G160">
+      <c r="G168">
         <v>3.846153846153846</v>
       </c>
     </row>

</xml_diff>